<commit_message>
Precinct layer with CT offpcap layer
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilongju/Dropbox/Study/GitHub/R_plot_by_neighborhood_ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilongju/Dropbox/Study/GitHub/VNSNY-UPENN-ABMS-Study-R-Map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ctuniq</t>
   </si>
@@ -195,12 +195,21 @@
   </si>
   <si>
     <t>showPercentage</t>
+  </si>
+  <si>
+    <t>major offense per capita</t>
+  </si>
+  <si>
+    <t>majoffpc</t>
+  </si>
+  <si>
+    <t>Crime data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -245,6 +254,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -572,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,14 +851,28 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Before mega code optimization
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-2740" windowWidth="25600" windowHeight="16160" tabRatio="500"/>
+    <workbookView xWindow="-8420" yWindow="-28360" windowWidth="51200" windowHeight="28360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>ctuniq</t>
   </si>
@@ -200,16 +200,259 @@
     <t>major offense per capita</t>
   </si>
   <si>
-    <t>majoffpc</t>
-  </si>
-  <si>
     <t>Crime data</t>
+  </si>
+  <si>
+    <t>num_er_08</t>
+  </si>
+  <si>
+    <t>er_charges_08</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_08</t>
+  </si>
+  <si>
+    <t>num_er_09</t>
+  </si>
+  <si>
+    <t>er_charges_09</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_09</t>
+  </si>
+  <si>
+    <t>num_er_10</t>
+  </si>
+  <si>
+    <t>er_charges_10</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_10</t>
+  </si>
+  <si>
+    <t>tot_er_pats</t>
+  </si>
+  <si>
+    <t>tot_er_charges</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_tot</t>
+  </si>
+  <si>
+    <t>num_pat_08</t>
+  </si>
+  <si>
+    <t>charges_08</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_08</t>
+  </si>
+  <si>
+    <t>num_pat_09</t>
+  </si>
+  <si>
+    <t>charges_09</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_09</t>
+  </si>
+  <si>
+    <t>num_pat_10</t>
+  </si>
+  <si>
+    <t>charges_10</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_10</t>
+  </si>
+  <si>
+    <t>tot_pats</t>
+  </si>
+  <si>
+    <t>tot_charges</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_tot</t>
+  </si>
+  <si>
+    <t>num_high_utils_08</t>
+  </si>
+  <si>
+    <t>num_high_utils_09</t>
+  </si>
+  <si>
+    <t>num_high_utils_10</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2008</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2009</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulated ER charges </t>
+  </si>
+  <si>
+    <t>Cumulated # of ER partients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pcap cumulated ER charges </t>
+  </si>
+  <si>
+    <t># of HC Patients in 2008</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2008</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2008</t>
+  </si>
+  <si>
+    <t># of HC Patients in 2009</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2009</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2009</t>
+  </si>
+  <si>
+    <t># of HC Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated # of HC partients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulated HC charges </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pcap cumulated HC charges </t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2008</t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2009</t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2010</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2008</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2009</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2010</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated ER charges for all years</t>
+  </si>
+  <si>
+    <t>Cumulated Number of ER Patients for all years</t>
+  </si>
+  <si>
+    <t>Per capita Cumulated ER charges for all years</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2008</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2008</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2008</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2009</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2009</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2009</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2010</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated HC charges for all years</t>
+  </si>
+  <si>
+    <t>Cumulated NumbHC of HC Patients for all years</t>
+  </si>
+  <si>
+    <t>PHC capita Cumulated HC charges for all years</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2008</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2009</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2010</t>
+  </si>
+  <si>
+    <t>offpcap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -583,16 +826,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="84.83203125" customWidth="1"/>
   </cols>
@@ -853,10 +1097,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -865,18 +1109,397 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After mega optimization and popups
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -200,9 +200,6 @@
     <t>major offense per capita</t>
   </si>
   <si>
-    <t>Crime data</t>
-  </si>
-  <si>
     <t>num_er_08</t>
   </si>
   <si>
@@ -447,6 +444,9 @@
   </si>
   <si>
     <t>offpcap</t>
+  </si>
+  <si>
+    <t>Pcap major offense</t>
   </si>
 </sst>
 </file>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1111,380 +1111,380 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert to see more variables
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilongju/Dropbox/Study/GitHub/VNSNY-UPENN-ABMS-Study-R-Map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966D5E75-25D4-1F4B-9AF8-243005C0D601}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F8D170-7145-3A47-B52F-A08287536016}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="22520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>ctuniq</t>
   </si>
@@ -223,15 +223,6 @@
   </si>
   <si>
     <t>Residents per square kilometer (based on 2000 Census)</t>
-  </si>
-  <si>
-    <t>avgChronCond</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chronic_count_08 averaged by the number of patients in a CT</t>
-  </si>
-  <si>
-    <t>Avg Chronic Counts 08</t>
   </si>
 </sst>
 </file>
@@ -612,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,46 +900,27 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Updated, organization map, variables"
This reverts commit 0852565301b4df77f79af68b105812223d5c7d8e.
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilongju/Dropbox/Study/GitHub/VNSNY-UPENN-ABMS-Study-R-Map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F8D170-7145-3A47-B52F-A08287536016}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="22520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8420" yWindow="-28360" windowWidth="51200" windowHeight="28360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>ctuniq</t>
   </si>
@@ -57,27 +56,51 @@
     <t>popdens</t>
   </si>
   <si>
+    <t>Population density: residents per square kilometer (based on 2000 Census)</t>
+  </si>
+  <si>
     <t>povrate</t>
   </si>
   <si>
+    <t>Poverty rate: proportion at or below federal poverty line (2000 Census)</t>
+  </si>
+  <si>
     <t>unemp</t>
   </si>
   <si>
+    <t>Unemployment rate: proportion of eligible workforce unemployed (2000 Census)</t>
+  </si>
+  <si>
     <t>busdens</t>
   </si>
   <si>
+    <t>Bus stop density: number of bus stops per square kilometer (from NYC MTA data)</t>
+  </si>
+  <si>
     <t>subdens</t>
   </si>
   <si>
+    <t>Subway stop density: number of subway stops/stations per square kilometer (from NYC MTA data)</t>
+  </si>
+  <si>
     <t>subacc</t>
   </si>
   <si>
+    <t>Subway access: binary variable derived from 'subdens' indicating whether or not there is a subway station within the census tract (1=yes; 0=no)</t>
+  </si>
+  <si>
     <t>intdens</t>
   </si>
   <si>
+    <t>Intersection density: number of intersections per square kilometer (derived from NYC Dept of City Planning Data, DCPLION)</t>
+  </si>
+  <si>
     <t>landind</t>
   </si>
   <si>
+    <t>Land use index: represents the mix of residential and commercial land use at tax lot level, aggregated to census tract level. Ranges from 0 to 1, where '0' indicates completely homogeneous (e.g. all tax lots in the census tract are either all residential or all commercial), and '1' indicates an even mix of commerical and residential. (Derived from NYC Dept of City Planning Data, PLUTO)</t>
+  </si>
+  <si>
     <t>nonres</t>
   </si>
   <si>
@@ -174,55 +197,256 @@
     <t>showPercentage</t>
   </si>
   <si>
+    <t>major offense per capita</t>
+  </si>
+  <si>
+    <t>num_er_08</t>
+  </si>
+  <si>
+    <t>er_charges_08</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_08</t>
+  </si>
+  <si>
+    <t>num_er_09</t>
+  </si>
+  <si>
+    <t>er_charges_09</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_09</t>
+  </si>
+  <si>
+    <t>num_er_10</t>
+  </si>
+  <si>
+    <t>er_charges_10</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_10</t>
+  </si>
+  <si>
+    <t>tot_er_pats</t>
+  </si>
+  <si>
+    <t>tot_er_charges</t>
+  </si>
+  <si>
+    <t>pcap_er_charges_tot</t>
+  </si>
+  <si>
+    <t>num_pat_08</t>
+  </si>
+  <si>
+    <t>charges_08</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_08</t>
+  </si>
+  <si>
+    <t>num_pat_09</t>
+  </si>
+  <si>
+    <t>charges_09</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_09</t>
+  </si>
+  <si>
+    <t>num_pat_10</t>
+  </si>
+  <si>
+    <t>charges_10</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_10</t>
+  </si>
+  <si>
+    <t>tot_pats</t>
+  </si>
+  <si>
+    <t>tot_charges</t>
+  </si>
+  <si>
+    <t>pcap_hc_charges_tot</t>
+  </si>
+  <si>
+    <t>num_high_utils_08</t>
+  </si>
+  <si>
+    <t>num_high_utils_09</t>
+  </si>
+  <si>
+    <t>num_high_utils_10</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2008</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2009</t>
+  </si>
+  <si>
+    <t># of ER Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Pcap ER charges in 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulated ER charges </t>
+  </si>
+  <si>
+    <t>Cumulated # of ER partients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pcap cumulated ER charges </t>
+  </si>
+  <si>
+    <t># of HC Patients in 2008</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2008</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2008</t>
+  </si>
+  <si>
+    <t># of HC Patients in 2009</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2009</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2009</t>
+  </si>
+  <si>
+    <t># of HC Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Pcap HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated # of HC partients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulated HC charges </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pcap cumulated HC charges </t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2008</t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2009</t>
+  </si>
+  <si>
+    <t># of high utilizers (top 20%) in 2010</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Total ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2008</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2009</t>
+  </si>
+  <si>
+    <t>Number of ER Patients in 2010</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2008</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2009</t>
+  </si>
+  <si>
+    <t>Per capita ER charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated ER charges for all years</t>
+  </si>
+  <si>
+    <t>Cumulated Number of ER Patients for all years</t>
+  </si>
+  <si>
+    <t>Per capita Cumulated ER charges for all years</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2008</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2008</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2008</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2009</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2009</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2009</t>
+  </si>
+  <si>
+    <t>NumbHC of HC Patients in 2010</t>
+  </si>
+  <si>
+    <t>Total HC charges in 2010</t>
+  </si>
+  <si>
+    <t>PHC capita HC charges in 2010</t>
+  </si>
+  <si>
+    <t>Cumulated HC charges for all years</t>
+  </si>
+  <si>
+    <t>Cumulated NumbHC of HC Patients for all years</t>
+  </si>
+  <si>
+    <t>PHC capita Cumulated HC charges for all years</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2008</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2009</t>
+  </si>
+  <si>
+    <t>Number of High Utilizers (top 20%) in 2010</t>
+  </si>
+  <si>
     <t>offpcap</t>
   </si>
   <si>
     <t>Pcap major offense</t>
-  </si>
-  <si>
-    <t>avg_er_charges_tot</t>
-  </si>
-  <si>
-    <t>avg_charges_tot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg ER charges </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg HC charges </t>
-  </si>
-  <si>
-    <t>Average Cumulated ER charges for all years</t>
-  </si>
-  <si>
-    <t>Average Cumulated HC charges for all years</t>
-  </si>
-  <si>
-    <t>Major offense per capita</t>
-  </si>
-  <si>
-    <t>The mix of residential and commercial land use at tax lot level, aggregated to census tract level. Ranges from 0 to 1, where '0' indicates completely homogeneous (e.g. all tax lots in the census tract are either all residential or all commercial), and '1' indicates an even mix of commerical and residential. (Derived from NYC Dept of City Planning Data, PLUTO)</t>
-  </si>
-  <si>
-    <t># of intersections per square kilometer (derived from NYC Dept of City Planning Data, DCPLION)</t>
-  </si>
-  <si>
-    <t>Binary variable derived from 'subdens' indicating whether or not there is a subway station within the census tract (1=yes; 0=no)</t>
-  </si>
-  <si>
-    <t># of subway stops/stations per square kilometer (from NYC MTA data)</t>
-  </si>
-  <si>
-    <t># of bus stops per square kilometer (from NYC MTA data)</t>
-  </si>
-  <si>
-    <t>Proportion of eligible workforce unemployed (2000 Census)</t>
-  </si>
-  <si>
-    <t>Proportion at or below federal poverty line (2000 Census)</t>
-  </si>
-  <si>
-    <t>Residents per square kilometer (based on 2000 Census)</t>
   </si>
 </sst>
 </file>
@@ -603,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,16 +843,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -680,203 +904,203 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -887,41 +1111,391 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>51</v>
+      <c r="A22" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>